<commit_message>
Modification stat "Tonnages répartition" Ajout gestion de produit ou CDT introuvable dans les transactions Laser Suppression catégories à l'impression des NC
</commit_message>
<xml_diff>
--- a/eVaSys.Server/Assets/Templates/NonConformite.xlsx
+++ b/eVaSys.Server/Assets/Templates/NonConformite.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sources\Repos\Valorplast\eValorplastWebApp\Assets\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sources\Repos\eVaSys\eVaSys.Server\Assets\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A35DF07-64BE-4D0C-A2E6-A197A564E6C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB945FF2-63B4-423D-B632-2F02DD448FC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="3840" windowWidth="45636" windowHeight="19452" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2112" yWindow="2520" windowWidth="25476" windowHeight="21300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NC" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>FICHE DE NON CONFORMITE</t>
   </si>
@@ -53,9 +53,6 @@
   </si>
   <si>
     <t>Type non-conformité</t>
-  </si>
-  <si>
-    <t>Catégories</t>
   </si>
   <si>
     <t>Retour de lot demandé</t>
@@ -657,7 +654,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C39"/>
+  <dimension ref="A2:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -688,7 +685,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="9"/>
@@ -749,14 +746,14 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="13"/>
@@ -795,129 +792,122 @@
       <c r="C20" s="10"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="10"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="16"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="16"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="14"/>
+      <c r="A23" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="9"/>
+      <c r="A24" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="10"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" s="2"/>
+      <c r="C25" s="17"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" s="4"/>
+      <c r="C26" s="13"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="9"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="10"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="18"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="14"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="17"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="B27" s="4"/>
-      <c r="C27" s="13"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="14"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" s="10"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="18"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="14"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="9"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="9"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="10"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="10"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="16"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="8"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="14"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="16"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="14"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="9"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" s="11"/>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="16"/>
+      <c r="A38" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>